<commit_message>
prueba con dos barridos
resultados iguales, decepcion emocional
</commit_message>
<xml_diff>
--- a/Robots/Fatima/model/old/reg0-180.xlsx
+++ b/Robots/Fatima/model/old/reg0-180.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\model\old\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wggm\Documents\GitHub\ISL-Maze-Solver-Robots\Robots\Fatima\model\old\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9665118F-5AB1-4088-8808-735EB67211AD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E130DCFC-5F8F-4406-A0CC-AF99880FF3F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="2448" windowWidth="17280" windowHeight="8964"/>
+    <workbookView xWindow="5760" yWindow="2448" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="reg0-45" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -854,11 +854,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B176"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="A177" sqref="A177:B221"/>
+    <sheetView tabSelected="1" topLeftCell="A330" workbookViewId="0">
+      <selection activeCell="A308" sqref="A308:B352"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2271,6 +2271,1414 @@
         <v>12</v>
       </c>
     </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A177">
+        <v>5</v>
+      </c>
+      <c r="B177">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A178">
+        <v>6</v>
+      </c>
+      <c r="B178">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A179">
+        <v>7</v>
+      </c>
+      <c r="B179">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A180">
+        <v>8</v>
+      </c>
+      <c r="B180">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A181">
+        <v>9</v>
+      </c>
+      <c r="B181">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A182">
+        <v>10</v>
+      </c>
+      <c r="B182">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A183">
+        <v>11</v>
+      </c>
+      <c r="B183">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A184">
+        <v>12</v>
+      </c>
+      <c r="B184">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A185">
+        <v>13</v>
+      </c>
+      <c r="B185">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A186">
+        <v>14</v>
+      </c>
+      <c r="B186">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A187">
+        <v>15</v>
+      </c>
+      <c r="B187">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A188">
+        <v>16</v>
+      </c>
+      <c r="B188">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A189">
+        <v>17</v>
+      </c>
+      <c r="B189">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A190">
+        <v>18</v>
+      </c>
+      <c r="B190">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A191">
+        <v>19</v>
+      </c>
+      <c r="B191">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A192">
+        <v>20</v>
+      </c>
+      <c r="B192">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A193">
+        <v>21</v>
+      </c>
+      <c r="B193">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A194">
+        <v>22</v>
+      </c>
+      <c r="B194">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A195">
+        <v>23</v>
+      </c>
+      <c r="B195">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A196">
+        <v>24</v>
+      </c>
+      <c r="B196">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A197">
+        <v>25</v>
+      </c>
+      <c r="B197">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A198">
+        <v>26</v>
+      </c>
+      <c r="B198">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A199">
+        <v>27</v>
+      </c>
+      <c r="B199">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A200">
+        <v>28</v>
+      </c>
+      <c r="B200">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A201">
+        <v>29</v>
+      </c>
+      <c r="B201">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A202">
+        <v>30</v>
+      </c>
+      <c r="B202">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A203">
+        <v>31</v>
+      </c>
+      <c r="B203">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A204">
+        <v>32</v>
+      </c>
+      <c r="B204">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A205">
+        <v>33</v>
+      </c>
+      <c r="B205">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A206">
+        <v>34</v>
+      </c>
+      <c r="B206">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A207">
+        <v>35</v>
+      </c>
+      <c r="B207">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A208">
+        <v>36</v>
+      </c>
+      <c r="B208">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A209">
+        <v>37</v>
+      </c>
+      <c r="B209">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A210">
+        <v>38</v>
+      </c>
+      <c r="B210">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A211">
+        <v>39</v>
+      </c>
+      <c r="B211">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A212">
+        <v>40</v>
+      </c>
+      <c r="B212">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A213">
+        <v>41</v>
+      </c>
+      <c r="B213">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A214">
+        <v>42</v>
+      </c>
+      <c r="B214">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A215">
+        <v>43</v>
+      </c>
+      <c r="B215">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A216">
+        <v>44</v>
+      </c>
+      <c r="B216">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A217">
+        <v>45</v>
+      </c>
+      <c r="B217">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A218">
+        <v>46</v>
+      </c>
+      <c r="B218">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A219">
+        <v>47</v>
+      </c>
+      <c r="B219">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A220">
+        <v>48</v>
+      </c>
+      <c r="B220">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A221">
+        <v>49</v>
+      </c>
+      <c r="B221">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A222">
+        <v>50</v>
+      </c>
+      <c r="B222">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A223">
+        <v>51</v>
+      </c>
+      <c r="B223">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A224">
+        <v>52</v>
+      </c>
+      <c r="B224">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A225">
+        <v>53</v>
+      </c>
+      <c r="B225">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A226">
+        <v>54</v>
+      </c>
+      <c r="B226">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A227">
+        <v>55</v>
+      </c>
+      <c r="B227">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A228">
+        <v>56</v>
+      </c>
+      <c r="B228">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A229">
+        <v>57</v>
+      </c>
+      <c r="B229">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A230">
+        <v>58</v>
+      </c>
+      <c r="B230">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A231">
+        <v>59</v>
+      </c>
+      <c r="B231">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A232">
+        <v>60</v>
+      </c>
+      <c r="B232">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A233">
+        <v>61</v>
+      </c>
+      <c r="B233">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A234">
+        <v>62</v>
+      </c>
+      <c r="B234">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A235">
+        <v>63</v>
+      </c>
+      <c r="B235">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A236">
+        <v>64</v>
+      </c>
+      <c r="B236">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A237">
+        <v>65</v>
+      </c>
+      <c r="B237">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A238">
+        <v>66</v>
+      </c>
+      <c r="B238">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A239">
+        <v>67</v>
+      </c>
+      <c r="B239">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A240">
+        <v>68</v>
+      </c>
+      <c r="B240">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A241">
+        <v>69</v>
+      </c>
+      <c r="B241">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A242">
+        <v>70</v>
+      </c>
+      <c r="B242">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A243">
+        <v>71</v>
+      </c>
+      <c r="B243">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A244">
+        <v>72</v>
+      </c>
+      <c r="B244">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A245">
+        <v>73</v>
+      </c>
+      <c r="B245">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A246">
+        <v>74</v>
+      </c>
+      <c r="B246">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A247">
+        <v>75</v>
+      </c>
+      <c r="B247">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A248">
+        <v>76</v>
+      </c>
+      <c r="B248">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A249">
+        <v>77</v>
+      </c>
+      <c r="B249">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A250">
+        <v>78</v>
+      </c>
+      <c r="B250">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A251">
+        <v>79</v>
+      </c>
+      <c r="B251">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A252">
+        <v>80</v>
+      </c>
+      <c r="B252">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A253">
+        <v>81</v>
+      </c>
+      <c r="B253">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A254">
+        <v>82</v>
+      </c>
+      <c r="B254">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A255">
+        <v>83</v>
+      </c>
+      <c r="B255">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A256">
+        <v>84</v>
+      </c>
+      <c r="B256">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A257">
+        <v>85</v>
+      </c>
+      <c r="B257">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A258">
+        <v>86</v>
+      </c>
+      <c r="B258">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A259">
+        <v>87</v>
+      </c>
+      <c r="B259">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A260">
+        <v>88</v>
+      </c>
+      <c r="B260">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A261">
+        <v>89</v>
+      </c>
+      <c r="B261">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A262">
+        <v>90</v>
+      </c>
+      <c r="B262">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A263">
+        <v>91</v>
+      </c>
+      <c r="B263">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A264">
+        <v>92</v>
+      </c>
+      <c r="B264">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A265">
+        <v>93</v>
+      </c>
+      <c r="B265">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A266">
+        <v>94</v>
+      </c>
+      <c r="B266">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A267">
+        <v>95</v>
+      </c>
+      <c r="B267">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A268">
+        <v>96</v>
+      </c>
+      <c r="B268">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A269">
+        <v>97</v>
+      </c>
+      <c r="B269">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A270">
+        <v>98</v>
+      </c>
+      <c r="B270">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A271">
+        <v>99</v>
+      </c>
+      <c r="B271">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A272">
+        <v>100</v>
+      </c>
+      <c r="B272">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A273">
+        <v>101</v>
+      </c>
+      <c r="B273">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A274">
+        <v>102</v>
+      </c>
+      <c r="B274">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A275">
+        <v>103</v>
+      </c>
+      <c r="B275">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A276">
+        <v>104</v>
+      </c>
+      <c r="B276">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A277">
+        <v>105</v>
+      </c>
+      <c r="B277">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A278">
+        <v>106</v>
+      </c>
+      <c r="B278">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A279">
+        <v>107</v>
+      </c>
+      <c r="B279">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A280">
+        <v>108</v>
+      </c>
+      <c r="B280">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A281">
+        <v>109</v>
+      </c>
+      <c r="B281">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A282">
+        <v>110</v>
+      </c>
+      <c r="B282">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A283">
+        <v>111</v>
+      </c>
+      <c r="B283">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A284">
+        <v>112</v>
+      </c>
+      <c r="B284">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A285">
+        <v>113</v>
+      </c>
+      <c r="B285">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A286">
+        <v>114</v>
+      </c>
+      <c r="B286">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A287">
+        <v>115</v>
+      </c>
+      <c r="B287">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A288">
+        <v>116</v>
+      </c>
+      <c r="B288">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A289">
+        <v>117</v>
+      </c>
+      <c r="B289">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A290">
+        <v>118</v>
+      </c>
+      <c r="B290">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A291">
+        <v>119</v>
+      </c>
+      <c r="B291">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A292">
+        <v>120</v>
+      </c>
+      <c r="B292">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A293">
+        <v>121</v>
+      </c>
+      <c r="B293">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A294">
+        <v>122</v>
+      </c>
+      <c r="B294">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A295">
+        <v>123</v>
+      </c>
+      <c r="B295">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A296">
+        <v>124</v>
+      </c>
+      <c r="B296">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A297">
+        <v>125</v>
+      </c>
+      <c r="B297">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A298">
+        <v>126</v>
+      </c>
+      <c r="B298">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A299">
+        <v>127</v>
+      </c>
+      <c r="B299">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A300">
+        <v>128</v>
+      </c>
+      <c r="B300">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A301">
+        <v>129</v>
+      </c>
+      <c r="B301">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A302">
+        <v>130</v>
+      </c>
+      <c r="B302">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A303">
+        <v>131</v>
+      </c>
+      <c r="B303">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A304">
+        <v>132</v>
+      </c>
+      <c r="B304">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A305">
+        <v>133</v>
+      </c>
+      <c r="B305">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A306">
+        <v>134</v>
+      </c>
+      <c r="B306">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A307">
+        <v>135</v>
+      </c>
+      <c r="B307">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A308">
+        <v>136</v>
+      </c>
+      <c r="B308">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A309">
+        <v>137</v>
+      </c>
+      <c r="B309">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A310">
+        <v>138</v>
+      </c>
+      <c r="B310">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A311">
+        <v>139</v>
+      </c>
+      <c r="B311">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A312">
+        <v>140</v>
+      </c>
+      <c r="B312">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A313">
+        <v>141</v>
+      </c>
+      <c r="B313">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A314">
+        <v>142</v>
+      </c>
+      <c r="B314">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A315">
+        <v>143</v>
+      </c>
+      <c r="B315">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A316">
+        <v>144</v>
+      </c>
+      <c r="B316">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A317">
+        <v>145</v>
+      </c>
+      <c r="B317">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A318">
+        <v>146</v>
+      </c>
+      <c r="B318">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A319">
+        <v>147</v>
+      </c>
+      <c r="B319">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A320">
+        <v>148</v>
+      </c>
+      <c r="B320">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A321">
+        <v>149</v>
+      </c>
+      <c r="B321">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A322">
+        <v>150</v>
+      </c>
+      <c r="B322">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A323">
+        <v>151</v>
+      </c>
+      <c r="B323">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A324">
+        <v>152</v>
+      </c>
+      <c r="B324">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A325">
+        <v>153</v>
+      </c>
+      <c r="B325">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A326">
+        <v>154</v>
+      </c>
+      <c r="B326">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A327">
+        <v>155</v>
+      </c>
+      <c r="B327">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A328">
+        <v>156</v>
+      </c>
+      <c r="B328">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A329">
+        <v>157</v>
+      </c>
+      <c r="B329">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A330">
+        <v>158</v>
+      </c>
+      <c r="B330">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A331">
+        <v>159</v>
+      </c>
+      <c r="B331">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A332">
+        <v>160</v>
+      </c>
+      <c r="B332">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A333">
+        <v>161</v>
+      </c>
+      <c r="B333">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A334">
+        <v>162</v>
+      </c>
+      <c r="B334">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A335">
+        <v>163</v>
+      </c>
+      <c r="B335">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A336">
+        <v>164</v>
+      </c>
+      <c r="B336">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A337">
+        <v>165</v>
+      </c>
+      <c r="B337">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A338">
+        <v>166</v>
+      </c>
+      <c r="B338">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A339">
+        <v>167</v>
+      </c>
+      <c r="B339">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A340">
+        <v>168</v>
+      </c>
+      <c r="B340">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A341">
+        <v>169</v>
+      </c>
+      <c r="B341">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A342">
+        <v>170</v>
+      </c>
+      <c r="B342">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A343">
+        <v>171</v>
+      </c>
+      <c r="B343">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A344">
+        <v>172</v>
+      </c>
+      <c r="B344">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A345">
+        <v>173</v>
+      </c>
+      <c r="B345">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A346">
+        <v>174</v>
+      </c>
+      <c r="B346">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A347">
+        <v>175</v>
+      </c>
+      <c r="B347">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A348">
+        <v>176</v>
+      </c>
+      <c r="B348">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A349">
+        <v>177</v>
+      </c>
+      <c r="B349">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A350">
+        <v>178</v>
+      </c>
+      <c r="B350">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A351">
+        <v>179</v>
+      </c>
+      <c r="B351">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A352">
+        <v>180</v>
+      </c>
+      <c r="B352">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>